<commit_message>
- Document + Slide.
</commit_message>
<xml_diff>
--- a/ smart-buy/Reports/TasksheetFinal.xlsx
+++ b/ smart-buy/Reports/TasksheetFinal.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="115">
   <si>
     <t>No.</t>
   </si>
@@ -462,13 +462,13 @@
     <t>Save to database</t>
   </si>
   <si>
-    <t>Upload file</t>
-  </si>
-  <si>
     <t>Add to cart</t>
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>Parse file</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,6 +711,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -731,12 +743,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1040,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1086,10 +1092,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="30">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1105,8 +1111,8 @@
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
@@ -1120,8 +1126,8 @@
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1135,8 +1141,8 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
@@ -1150,8 +1156,8 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1165,8 +1171,8 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1180,10 +1186,10 @@
       <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A8" s="31">
+      <c r="A8" s="35">
         <v>2</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1199,8 +1205,8 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="31"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="4" t="s">
         <v>35</v>
       </c>
@@ -1214,8 +1220,8 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="31"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
@@ -1229,8 +1235,8 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1244,8 +1250,8 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1259,11 +1265,11 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A13" s="31">
+      <c r="A13" s="35">
         <v>3</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="38" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="31" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2"/>
@@ -1274,9 +1280,9 @@
       <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A14" s="31"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="37" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="2"/>
@@ -1289,10 +1295,10 @@
       <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="37" t="s">
-        <v>113</v>
+      <c r="A15" s="35"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1304,10 +1310,10 @@
       <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="37" t="s">
-        <v>114</v>
+      <c r="A16" s="35"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="30" t="s">
+        <v>113</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1317,9 +1323,9 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="15.75">
-      <c r="A17" s="31"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="38" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="2"/>
@@ -1330,9 +1336,9 @@
       <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="31"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="37" t="s">
+      <c r="A18" s="35"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1345,9 +1351,9 @@
       <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="31"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="37" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="30" t="s">
         <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1360,9 +1366,9 @@
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="31"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="37" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="30" t="s">
         <v>67</v>
       </c>
       <c r="D20" s="2"/>
@@ -1375,9 +1381,9 @@
       <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="31"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="38" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="31" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="2"/>
@@ -1388,68 +1394,68 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="31"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="37" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="32" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G22" s="2"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="31"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A23" s="35"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="37" t="s">
-        <v>114</v>
+      <c r="A24" s="35"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="33" t="s">
+        <v>110</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="31"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A25" s="35"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="31"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="6" t="s">
-        <v>42</v>
+      <c r="A26" s="35"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1461,14 +1467,12 @@
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="31"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A27" s="35"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1476,10 +1480,10 @@
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="31"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="7" t="s">
-        <v>44</v>
+      <c r="A28" s="35"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -1491,10 +1495,10 @@
       <c r="I28" s="13"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="31"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="7" t="s">
-        <v>45</v>
+      <c r="A29" s="35"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1505,17 +1509,15 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="32">
-        <v>4</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="2"/>
+    <row r="30" spans="1:9" ht="15.75">
+      <c r="A30" s="35"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1523,10 +1525,10 @@
       <c r="I30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="9" t="s">
-        <v>47</v>
+      <c r="A31" s="35"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1538,29 +1540,31 @@
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="2"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>6</v>
-      </c>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A33" s="36">
+        <v>4</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1568,12 +1572,14 @@
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="2"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1581,27 +1587,29 @@
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="2"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1609,25 +1617,23 @@
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="28" t="s">
-        <v>51</v>
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G37" s="2"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="23" t="s">
-        <v>52</v>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -1639,55 +1645,53 @@
       <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="23" t="s">
-        <v>53</v>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G39" s="2"/>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="23" t="s">
-        <v>54</v>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="33"/>
-      <c r="B41" s="33"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1699,25 +1703,25 @@
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1729,25 +1733,25 @@
       <c r="I44" s="13"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="30"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
@@ -1759,40 +1763,40 @@
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="22"/>
-      <c r="B47" s="33"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="22"/>
-      <c r="B48" s="33"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="37"/>
       <c r="C48" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="2"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="22"/>
-      <c r="B49" s="33"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -1805,9 +1809,9 @@
     </row>
     <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="22"/>
-      <c r="B50" s="33"/>
+      <c r="B50" s="37"/>
       <c r="C50" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
@@ -1820,22 +1824,24 @@
     </row>
     <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="22"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="24" t="s">
-        <v>12</v>
+      <c r="B51" s="37"/>
+      <c r="C51" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="G51" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="22"/>
-      <c r="B52" s="33"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
@@ -1848,69 +1854,67 @@
     </row>
     <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="22"/>
-      <c r="B53" s="33"/>
+      <c r="B53" s="37"/>
       <c r="C53" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G53" s="2"/>
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="22"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="23" t="s">
-        <v>67</v>
+      <c r="B54" s="37"/>
+      <c r="C54" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
       <c r="A55" s="22"/>
-      <c r="B55" s="33"/>
+      <c r="B55" s="37"/>
       <c r="C55" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E55" s="2"/>
-      <c r="F55" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
       <c r="A56" s="22"/>
-      <c r="B56" s="33"/>
+      <c r="B56" s="37"/>
       <c r="C56" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
       <c r="A57" s="22"/>
-      <c r="B57" s="33"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1923,56 +1927,58 @@
     </row>
     <row r="58" spans="1:9" ht="15.75">
       <c r="A58" s="22"/>
-      <c r="B58" s="33"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G58" s="2"/>
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="22"/>
-      <c r="B59" s="33"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G59" s="2"/>
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="22"/>
-      <c r="B60" s="33"/>
+      <c r="B60" s="37"/>
       <c r="C60" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G60" s="2"/>
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
       <c r="A61" s="22"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D61" s="2"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -1981,97 +1987,97 @@
     </row>
     <row r="62" spans="1:9" ht="15.75">
       <c r="A62" s="22"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D62" s="2"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G62" s="2"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
       <c r="A63" s="22"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D63" s="2"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E63" s="2"/>
-      <c r="F63" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
       <c r="A64" s="22"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="26" t="s">
-        <v>77</v>
+      <c r="B64" s="37"/>
+      <c r="C64" s="25" t="s">
+        <v>74</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G64" s="2"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="1:9" ht="15.75">
       <c r="A65" s="22"/>
-      <c r="B65" s="33"/>
+      <c r="B65" s="37"/>
       <c r="C65" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
     <row r="66" spans="1:9" ht="15.75">
       <c r="A66" s="22"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="25" t="s">
-        <v>79</v>
+      <c r="B66" s="37"/>
+      <c r="C66" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
+      <c r="F66" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G66" s="2"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
     <row r="67" spans="1:9" ht="15.75">
       <c r="A67" s="22"/>
-      <c r="B67" s="33"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
+      <c r="G67" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
     <row r="68" spans="1:9" ht="15.75">
       <c r="A68" s="22"/>
-      <c r="B68" s="33"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2084,9 +2090,9 @@
     </row>
     <row r="69" spans="1:9" ht="15.75">
       <c r="A69" s="22"/>
-      <c r="B69" s="33"/>
+      <c r="B69" s="37"/>
       <c r="C69" s="25" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2097,9 +2103,9 @@
     </row>
     <row r="70" spans="1:9" ht="15.75">
       <c r="A70" s="22"/>
-      <c r="B70" s="33"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>6</v>
@@ -2112,28 +2118,24 @@
     </row>
     <row r="71" spans="1:9" ht="15.75">
       <c r="A71" s="22"/>
-      <c r="B71" s="30"/>
+      <c r="B71" s="37"/>
       <c r="C71" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D71" s="2"/>
       <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
+      <c r="F71" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G71" s="2"/>
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A72" s="34">
-        <v>5</v>
-      </c>
-      <c r="B72" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72" s="29" t="s">
-        <v>80</v>
+    <row r="72" spans="1:9" ht="15.75">
+      <c r="A72" s="22"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -2143,10 +2145,10 @@
       <c r="I72" s="13"/>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="35"/>
-      <c r="B73" s="33"/>
-      <c r="C73" s="9" t="s">
-        <v>84</v>
+      <c r="A73" s="22"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="26" t="s">
+        <v>82</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>6</v>
@@ -2155,55 +2157,51 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="13"/>
-      <c r="I73" s="13">
-        <v>1</v>
-      </c>
+      <c r="I73" s="13"/>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="35"/>
-      <c r="B74" s="33"/>
-      <c r="C74" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D74" s="2"/>
+      <c r="A74" s="22"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G74" s="2"/>
       <c r="H74" s="13"/>
-      <c r="I74" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="15.75">
-      <c r="A75" s="35"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="9" t="s">
-        <v>71</v>
+      <c r="I74" s="13"/>
+    </row>
+    <row r="75" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A75" s="38">
+        <v>5</v>
+      </c>
+      <c r="B75" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="29" t="s">
+        <v>80</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
-      <c r="F75" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="13"/>
-      <c r="I75" s="13">
-        <v>2</v>
-      </c>
+      <c r="I75" s="13"/>
     </row>
     <row r="76" spans="1:9" ht="15.75">
-      <c r="A76" s="35"/>
-      <c r="B76" s="33"/>
+      <c r="A76" s="39"/>
+      <c r="B76" s="37"/>
       <c r="C76" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D76" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E76" s="2"/>
-      <c r="F76" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="13"/>
       <c r="I76" s="13">
@@ -2211,27 +2209,27 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="15.75">
-      <c r="A77" s="35"/>
-      <c r="B77" s="33"/>
+      <c r="A77" s="39"/>
+      <c r="B77" s="37"/>
       <c r="C77" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
+      <c r="G77" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H77" s="13"/>
       <c r="I77" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="15.75">
-      <c r="A78" s="35"/>
-      <c r="B78" s="33"/>
+      <c r="A78" s="39"/>
+      <c r="B78" s="37"/>
       <c r="C78" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -2245,10 +2243,10 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="15.75">
-      <c r="A79" s="35"/>
-      <c r="B79" s="33"/>
+      <c r="A79" s="39"/>
+      <c r="B79" s="37"/>
       <c r="C79" s="9" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -2262,10 +2260,10 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="15.75">
-      <c r="A80" s="35"/>
-      <c r="B80" s="33"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="37"/>
       <c r="C80" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
@@ -2275,48 +2273,48 @@
       <c r="G80" s="2"/>
       <c r="H80" s="13"/>
       <c r="I80" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="35"/>
-      <c r="B81" s="33"/>
+      <c r="A81" s="39"/>
+      <c r="B81" s="37"/>
       <c r="C81" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D81" s="2"/>
       <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
+      <c r="F81" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G81" s="2"/>
       <c r="H81" s="13"/>
       <c r="I81" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="35"/>
-      <c r="B82" s="33"/>
+      <c r="A82" s="39"/>
+      <c r="B82" s="37"/>
       <c r="C82" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D82" s="2"/>
       <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
+      <c r="F82" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G82" s="2"/>
       <c r="H82" s="13"/>
       <c r="I82" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="35"/>
-      <c r="B83" s="33"/>
+      <c r="A83" s="39"/>
+      <c r="B83" s="37"/>
       <c r="C83" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>6</v>
@@ -2326,146 +2324,146 @@
       <c r="G83" s="2"/>
       <c r="H83" s="13"/>
       <c r="I83" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="35"/>
-      <c r="B84" s="33"/>
-      <c r="C84" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D84" s="2"/>
+      <c r="A84" s="39"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
+      <c r="I84" s="13">
+        <v>5</v>
+      </c>
     </row>
     <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="35"/>
-      <c r="B85" s="33"/>
-      <c r="C85" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D85" s="2"/>
+      <c r="A85" s="39"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G85" s="2"/>
       <c r="H85" s="13"/>
       <c r="I85" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="35"/>
-      <c r="B86" s="33"/>
-      <c r="C86" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D86" s="2"/>
+      <c r="A86" s="39"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G86" s="2"/>
       <c r="H86" s="13"/>
       <c r="I86" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="35"/>
-      <c r="B87" s="33"/>
-      <c r="C87" s="28" t="s">
-        <v>111</v>
+      <c r="A87" s="39"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G87" s="2"/>
       <c r="H87" s="13"/>
-      <c r="I87" s="13">
-        <v>2</v>
-      </c>
+      <c r="I87" s="13"/>
     </row>
     <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="35"/>
-      <c r="B88" s="33"/>
-      <c r="C88" s="9" t="s">
-        <v>90</v>
+      <c r="A88" s="39"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
-      <c r="F88" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H88" s="13"/>
       <c r="I88" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15.75">
-      <c r="A89" s="35"/>
-      <c r="B89" s="33"/>
-      <c r="C89" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A89" s="39"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
+      <c r="G89" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H89" s="13"/>
       <c r="I89" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15.75">
-      <c r="A90" s="35"/>
-      <c r="B90" s="33"/>
-      <c r="C90" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A90" s="39"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
+      <c r="G90" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H90" s="13"/>
       <c r="I90" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15.75">
-      <c r="A91" s="35"/>
-      <c r="B91" s="33"/>
+      <c r="A91" s="39"/>
+      <c r="B91" s="37"/>
       <c r="C91" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F91" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" s="2"/>
       <c r="H91" s="13"/>
       <c r="I91" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15.75">
-      <c r="A92" s="35"/>
-      <c r="B92" s="33"/>
+      <c r="A92" s="39"/>
+      <c r="B92" s="37"/>
       <c r="C92" s="9" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>6</v>
@@ -2479,46 +2477,50 @@
       </c>
     </row>
     <row r="93" spans="1:9" ht="15.75">
-      <c r="A93" s="36"/>
-      <c r="B93" s="33"/>
+      <c r="A93" s="39"/>
+      <c r="B93" s="37"/>
       <c r="C93" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D93" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
-      <c r="G93" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G93" s="2"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15.75">
-      <c r="A94" s="21"/>
-      <c r="B94" s="33"/>
-      <c r="C94" s="29" t="s">
-        <v>81</v>
+      <c r="A94" s="39"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
+      <c r="G94" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
+      <c r="I94" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="95" spans="1:9" ht="15.75">
-      <c r="A95" s="21"/>
-      <c r="B95" s="33"/>
+      <c r="A95" s="39"/>
+      <c r="B95" s="37"/>
       <c r="C95" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D95" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E95" s="2"/>
-      <c r="F95" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="13"/>
       <c r="I95" s="13">
@@ -2526,44 +2528,40 @@
       </c>
     </row>
     <row r="96" spans="1:9" ht="15.75">
-      <c r="A96" s="21"/>
-      <c r="B96" s="33"/>
+      <c r="A96" s="40"/>
+      <c r="B96" s="37"/>
       <c r="C96" s="9" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
-      <c r="F96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H96" s="13"/>
       <c r="I96" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15.75">
       <c r="A97" s="21"/>
-      <c r="B97" s="33"/>
-      <c r="C97" s="9" t="s">
-        <v>86</v>
+      <c r="B97" s="37"/>
+      <c r="C97" s="29" t="s">
+        <v>81</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
-      <c r="F97" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="13"/>
-      <c r="I97" s="13">
-        <v>1</v>
-      </c>
+      <c r="I97" s="13"/>
     </row>
     <row r="98" spans="1:9" ht="15.75">
       <c r="A98" s="21"/>
-      <c r="B98" s="33"/>
+      <c r="B98" s="37"/>
       <c r="C98" s="9" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -2573,14 +2571,14 @@
       <c r="G98" s="2"/>
       <c r="H98" s="13"/>
       <c r="I98" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.75">
       <c r="A99" s="21"/>
-      <c r="B99" s="33"/>
+      <c r="B99" s="37"/>
       <c r="C99" s="9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -2590,14 +2588,14 @@
       <c r="G99" s="2"/>
       <c r="H99" s="13"/>
       <c r="I99" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15.75">
       <c r="A100" s="21"/>
-      <c r="B100" s="33"/>
+      <c r="B100" s="37"/>
       <c r="C100" s="9" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -2607,14 +2605,14 @@
       <c r="G100" s="2"/>
       <c r="H100" s="13"/>
       <c r="I100" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="15.75">
       <c r="A101" s="21"/>
-      <c r="B101" s="33"/>
+      <c r="B101" s="37"/>
       <c r="C101" s="9" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -2629,37 +2627,43 @@
     </row>
     <row r="102" spans="1:9" ht="15.75">
       <c r="A102" s="21"/>
-      <c r="B102" s="33"/>
-      <c r="C102" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B102" s="37"/>
+      <c r="C102" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D102" s="2"/>
       <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
+      <c r="F102" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G102" s="2"/>
       <c r="H102" s="13"/>
-      <c r="I102" s="13"/>
+      <c r="I102" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:9" ht="15.75">
       <c r="A103" s="21"/>
-      <c r="B103" s="33"/>
-      <c r="C103" s="29" t="s">
-        <v>97</v>
+      <c r="B103" s="37"/>
+      <c r="C103" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
+      <c r="F103" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G103" s="2"/>
       <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
+      <c r="I103" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="104" spans="1:9" ht="15.75">
       <c r="A104" s="21"/>
-      <c r="B104" s="33"/>
+      <c r="B104" s="37"/>
       <c r="C104" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -2668,90 +2672,92 @@
       </c>
       <c r="G104" s="2"/>
       <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
+      <c r="I104" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="105" spans="1:9" ht="15.75">
       <c r="A105" s="21"/>
-      <c r="B105" s="33"/>
-      <c r="C105" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D105" s="2"/>
+      <c r="B105" s="37"/>
+      <c r="C105" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E105" s="2"/>
-      <c r="F105" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="13"/>
       <c r="I105" s="13"/>
     </row>
     <row r="106" spans="1:9" ht="15.75">
       <c r="A106" s="21"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="9" t="s">
-        <v>100</v>
+      <c r="B106" s="37"/>
+      <c r="C106" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
-      <c r="G106" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G106" s="2"/>
       <c r="H106" s="13"/>
       <c r="I106" s="13"/>
     </row>
     <row r="107" spans="1:9" ht="15.75">
-      <c r="A107" s="34">
-        <v>6</v>
-      </c>
-      <c r="B107" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="29" t="s">
-        <v>13</v>
+      <c r="A107" s="21"/>
+      <c r="B107" s="37"/>
+      <c r="C107" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
+      <c r="F107" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G107" s="2"/>
       <c r="H107" s="13"/>
       <c r="I107" s="13"/>
     </row>
     <row r="108" spans="1:9" ht="15.75">
-      <c r="A108" s="35"/>
-      <c r="B108" s="33"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="37"/>
       <c r="C108" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D108" s="2"/>
       <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G108" s="2"/>
       <c r="H108" s="13"/>
       <c r="I108" s="13"/>
     </row>
     <row r="109" spans="1:9" ht="15.75">
-      <c r="A109" s="35"/>
-      <c r="B109" s="33"/>
+      <c r="A109" s="21"/>
+      <c r="B109" s="34"/>
       <c r="C109" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
+      <c r="G109" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H109" s="13"/>
       <c r="I109" s="13"/>
     </row>
     <row r="110" spans="1:9" ht="15.75">
-      <c r="A110" s="35"/>
-      <c r="B110" s="33"/>
-      <c r="C110" s="27" t="s">
-        <v>103</v>
+      <c r="A110" s="38">
+        <v>6</v>
+      </c>
+      <c r="B110" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="29" t="s">
+        <v>13</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
@@ -2761,10 +2767,10 @@
       <c r="I110" s="13"/>
     </row>
     <row r="111" spans="1:9" ht="15.75">
-      <c r="A111" s="35"/>
-      <c r="B111" s="33"/>
-      <c r="C111" s="28" t="s">
-        <v>104</v>
+      <c r="A111" s="39"/>
+      <c r="B111" s="37"/>
+      <c r="C111" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>6</v>
@@ -2776,25 +2782,25 @@
       <c r="I111" s="13"/>
     </row>
     <row r="112" spans="1:9" ht="15.75">
-      <c r="A112" s="35"/>
-      <c r="B112" s="33"/>
-      <c r="C112" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D112" s="2"/>
+      <c r="A112" s="39"/>
+      <c r="B112" s="37"/>
+      <c r="C112" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E112" s="2"/>
-      <c r="F112" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F112" s="2"/>
       <c r="G112" s="2"/>
       <c r="H112" s="13"/>
       <c r="I112" s="13"/>
     </row>
     <row r="113" spans="1:9" ht="15.75">
-      <c r="A113" s="35"/>
-      <c r="B113" s="33"/>
-      <c r="C113" s="29" t="s">
-        <v>106</v>
+      <c r="A113" s="39"/>
+      <c r="B113" s="37"/>
+      <c r="C113" s="27" t="s">
+        <v>103</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
@@ -2804,25 +2810,25 @@
       <c r="I113" s="13"/>
     </row>
     <row r="114" spans="1:9" ht="15.75">
-      <c r="A114" s="35"/>
-      <c r="B114" s="33"/>
+      <c r="A114" s="39"/>
+      <c r="B114" s="37"/>
       <c r="C114" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="D114" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E114" s="2"/>
-      <c r="F114" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F114" s="2"/>
       <c r="G114" s="2"/>
       <c r="H114" s="13"/>
       <c r="I114" s="13"/>
     </row>
     <row r="115" spans="1:9" ht="15.75">
-      <c r="A115" s="35"/>
-      <c r="B115" s="33"/>
+      <c r="A115" s="39"/>
+      <c r="B115" s="37"/>
       <c r="C115" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
@@ -2834,116 +2840,159 @@
       <c r="I115" s="13"/>
     </row>
     <row r="116" spans="1:9" ht="15.75">
-      <c r="A116" s="36"/>
-      <c r="B116" s="30"/>
-      <c r="C116" s="28" t="s">
-        <v>109</v>
+      <c r="A116" s="39"/>
+      <c r="B116" s="37"/>
+      <c r="C116" s="29" t="s">
+        <v>106</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
-      <c r="G116" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G116" s="2"/>
       <c r="H116" s="13"/>
       <c r="I116" s="13"/>
     </row>
-    <row r="117" spans="1:9">
-      <c r="C117" s="1"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="I117" s="3"/>
-    </row>
-    <row r="118" spans="1:9">
-      <c r="C118" s="1"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="I118" s="3"/>
-    </row>
-    <row r="119" spans="1:9">
-      <c r="B119" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="I119" s="3"/>
-    </row>
-    <row r="120" spans="1:9" ht="60">
-      <c r="B120" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C120" s="4">
-        <v>1</v>
-      </c>
+    <row r="117" spans="1:9" ht="15.75">
+      <c r="A117" s="39"/>
+      <c r="B117" s="37"/>
+      <c r="C117" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G117" s="2"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+    </row>
+    <row r="118" spans="1:9" ht="15.75">
+      <c r="A118" s="39"/>
+      <c r="B118" s="37"/>
+      <c r="C118" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G118" s="2"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+    </row>
+    <row r="119" spans="1:9" ht="15.75">
+      <c r="A119" s="40"/>
+      <c r="B119" s="34"/>
+      <c r="C119" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="C120" s="1"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="I120" s="3"/>
     </row>
-    <row r="121" spans="1:9" ht="30">
-      <c r="B121" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C121" s="20">
-        <v>2</v>
-      </c>
+    <row r="121" spans="1:9">
+      <c r="C121" s="1"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
       <c r="I121" s="3"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
-      <c r="B122" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C122" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="30">
+    <row r="122" spans="1:9">
+      <c r="B122" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="I122" s="3"/>
+    </row>
+    <row r="123" spans="1:9" ht="60">
       <c r="B123" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C123" s="20">
-        <v>4</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C123" s="4">
+        <v>1</v>
+      </c>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="I123" s="3"/>
     </row>
     <row r="124" spans="1:9" ht="30">
       <c r="B124" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C124" s="20">
+        <v>2</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+      <c r="I124" s="3"/>
+    </row>
+    <row r="125" spans="1:9" ht="30">
+      <c r="B125" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C125" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="30">
+      <c r="B126" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="30">
+      <c r="B127" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C124" s="20">
+      <c r="C127" s="20">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A107:A116"/>
-    <mergeCell ref="B107:B116"/>
-    <mergeCell ref="A72:A93"/>
-    <mergeCell ref="A30:A45"/>
-    <mergeCell ref="B30:B71"/>
-    <mergeCell ref="B72:B106"/>
+    <mergeCell ref="A110:A119"/>
+    <mergeCell ref="B110:B119"/>
+    <mergeCell ref="A75:A96"/>
+    <mergeCell ref="A33:A48"/>
+    <mergeCell ref="B33:B74"/>
+    <mergeCell ref="B75:B109"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A13:A29"/>
+    <mergeCell ref="A13:A32"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B29"/>
+    <mergeCell ref="B12:B32"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G119">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G122">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>